<commit_message>
Update populations with 2016 previsions ()
</commit_message>
<xml_diff>
--- a/Update_WID_external_data.xlsx
+++ b/Update_WID_external_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="139">
   <si>
     <t>URL</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>https://esa.un.org/unpd/wpp/DVD/Files/1_Indicators%20(Standard)/ASCII_FILES/WPP2015_DB04_Population_By_Age_Annual.zip</t>
+  </si>
+  <si>
+    <t>WPP2015_DB04_Population_By_Age_Annual.csv</t>
+  </si>
+  <si>
+    <t>UN WPP Population previsions</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1030,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,9 +1549,15 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>134</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>135</v>

</xml_diff>